<commit_message>
Project 1 code till Sep 5th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\010LivetechWS\AdactinHybridFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72213FAB-BF30-4F49-AE3B-E51321070D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3BEAC2-8EFE-45E1-9A33-C2193B0B65C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0553831A-864E-45A9-94AF-A275648CAEA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>TC001</t>
   </si>
@@ -75,6 +75,39 @@
   </si>
   <si>
     <t>Enter Username</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Number of Rooms</t>
+  </si>
+  <si>
+    <t>2 - Two</t>
+  </si>
+  <si>
+    <t>Check In Date</t>
+  </si>
+  <si>
+    <t>Check Out Date</t>
+  </si>
+  <si>
+    <t>06/09/2024</t>
+  </si>
+  <si>
+    <t>07/09/2024</t>
+  </si>
+  <si>
+    <t>Adactin.com - Select Hotel</t>
+  </si>
+  <si>
+    <t>expectedTitle2</t>
   </si>
 </sst>
 </file>
@@ -117,9 +150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A447A611-C760-4A4B-B907-164454BD7B46}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>
@@ -446,10 +480,15 @@
     <col min="2" max="2" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -491,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -505,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -513,12 +552,70 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>